<commit_message>
Formatting updates; PNG export
</commit_message>
<xml_diff>
--- a/survey/clusters/QQ9-14_5CL_analysis_FINAL.xlsx
+++ b/survey/clusters/QQ9-14_5CL_analysis_FINAL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="10500" windowHeight="17208" activeTab="6"/>
+    <workbookView xWindow="192" yWindow="48" windowWidth="10500" windowHeight="17208"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,11 @@
     <sheet name="Cluster 5" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Cluster 1'!$A$1:$AJ$60</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Cluster 2'!$A$1:$AH$61</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Cluster 3'!$A$1:$AH$61</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Cluster 4'!$A$1:$AJ$62</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Cluster 5'!$A$1:$AH$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Cluster 1'!$B$2:$AK$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Cluster 2'!$B$2:$AJ$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Cluster 3'!$B$2:$AJ$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Cluster 4'!$B$2:$AJ$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Cluster 5'!$B$2:$AJ$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$R$83</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$U$39</definedName>
   </definedNames>
@@ -608,34 +608,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177052</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>4034</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect r="6604" b="9168"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="2371612"/>
-          <a:ext cx="7780020" cy="10068262"/>
+          <a:off x="12923520" y="426720"/>
+          <a:ext cx="7543800" cy="9494520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,16 +647,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>181494</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>501534</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>173916</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -666,14 +667,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect r="7480" b="6133"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6277494" y="0"/>
-          <a:ext cx="8048106" cy="10415196"/>
+          <a:off x="5987934" y="68580"/>
+          <a:ext cx="7446126" cy="9776460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -684,34 +686,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>28688</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect r="18022" b="19415"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13357860" y="0"/>
-          <a:ext cx="8077200" cy="10452848"/>
+          <a:off x="0" y="1106692"/>
+          <a:ext cx="6377940" cy="8113508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -727,34 +730,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177052</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>4033</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect r="7736" b="10699"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="2371612"/>
-          <a:ext cx="7780020" cy="10068261"/>
+          <a:off x="13411200" y="594360"/>
+          <a:ext cx="7452360" cy="9334500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -766,15 +770,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>181494</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>326274</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>173916</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -785,14 +789,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect r="8237" b="7523"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6277494" y="0"/>
-          <a:ext cx="8048105" cy="10415196"/>
+          <a:off x="6422274" y="373380"/>
+          <a:ext cx="7385166" cy="9631680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,34 +808,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>17032</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>28687</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect r="16259" b="22518"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13357860" y="0"/>
-          <a:ext cx="8077200" cy="10452847"/>
+          <a:off x="0" y="2211592"/>
+          <a:ext cx="6515100" cy="7801088"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -846,34 +852,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177052</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472439</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>4033</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect r="5849" b="10699"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="2371612"/>
-          <a:ext cx="7780019" cy="10068261"/>
+          <a:off x="13403580" y="533400"/>
+          <a:ext cx="7604760" cy="9334500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -885,15 +892,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>181494</xdr:colOff>
+      <xdr:colOff>448194</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>167641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>173915</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -904,14 +911,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect r="10794" b="8620"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6277494" y="1"/>
-          <a:ext cx="8048105" cy="10415194"/>
+          <a:off x="6544194" y="167641"/>
+          <a:ext cx="7179426" cy="9517379"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -922,34 +930,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>99059</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>28687</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect r="15279" b="23199"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13357860" y="0"/>
-          <a:ext cx="8077199" cy="10452847"/>
+          <a:off x="7620" y="1624852"/>
+          <a:ext cx="6591300" cy="7732508"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -965,34 +974,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1793</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>502919</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>11652</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect r="6415" b="11063"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38100" y="2379233"/>
-          <a:ext cx="7780019" cy="10068259"/>
+          <a:off x="13456920" y="441961"/>
+          <a:ext cx="7559040" cy="9296399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1004,15 +1014,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>181494</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>532014</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>304798</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>173915</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>45718</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1023,14 +1033,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect b="7669"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6277494" y="1"/>
-          <a:ext cx="8048104" cy="10415194"/>
+          <a:off x="6628014" y="198121"/>
+          <a:ext cx="8048104" cy="9616439"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1041,34 +1052,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>99059</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>28686</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect t="2480" r="17629" b="22669"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13357860" y="1"/>
-          <a:ext cx="8077199" cy="10452845"/>
+          <a:off x="312420" y="2072640"/>
+          <a:ext cx="6408420" cy="7536180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1084,34 +1096,35 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177053</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472438</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>4032</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="5472" r="7358" b="10553"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="2371613"/>
-          <a:ext cx="7780018" cy="10068259"/>
+          <a:off x="13510260" y="312421"/>
+          <a:ext cx="7040880" cy="9349739"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1123,15 +1136,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>181494</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>304798</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>173914</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1142,14 +1155,15 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="3994" r="10225" b="7596"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6277494" y="1"/>
-          <a:ext cx="8048104" cy="10415193"/>
+          <a:off x="6454140" y="220981"/>
+          <a:ext cx="6903720" cy="9624059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1160,34 +1174,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>99058</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>28686</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Employment_QQ_9_14_5CL_1-2.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Demographics_QQ_9_14_5CL_1-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect t="3691" r="18217" b="20853"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13357860" y="1"/>
-          <a:ext cx="8077198" cy="10452845"/>
+          <a:off x="167640" y="1882140"/>
+          <a:ext cx="6362700" cy="7597140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1489,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4248,56 +4263,60 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AJ60"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="8" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:2" s="8" customFormat="1"/>
+    <row r="2" spans="2:2" s="8" customFormat="1">
+      <c r="B2" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="8" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="9" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="9" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="9" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="8" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="8" t="s">
+    <row r="55" spans="6:6">
+      <c r="F55" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="6" t="s">
+    <row r="56" spans="6:6">
+      <c r="F56" s="6" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4313,10 +4332,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="B2:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AH61"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="Y73" sqref="Y73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4324,79 +4343,79 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="2:2">
+      <c r="B2" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="8" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="9" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="9" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="2:2">
+      <c r="B9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="2:2">
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="2:2">
+      <c r="B11" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="2:2">
+      <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="2:2">
+      <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="8" t="s">
+    <row r="56" spans="9:9">
+      <c r="I56" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="6" t="s">
+    <row r="57" spans="9:9">
+      <c r="I57" s="6" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="43" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4406,10 +4425,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="B2:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AH61"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4417,59 +4436,59 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="2:2">
+      <c r="B2" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="9" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="2:2">
+      <c r="B9" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="8" t="s">
+    <row r="54" spans="9:9">
+      <c r="I54" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="6" t="s">
+    <row r="55" spans="9:9">
+      <c r="I55" s="6" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="43" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4479,10 +4498,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="B2:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AJ62"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4490,64 +4509,64 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="2:2">
+      <c r="B2" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="9" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="9" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="9" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="8" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="2:2">
+      <c r="B9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="2:2">
+      <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="8" t="s">
+    <row r="55" spans="8:8">
+      <c r="H55" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="6" t="s">
+    <row r="56" spans="8:8">
+      <c r="H56" s="6" t="s">
         <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="41" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4557,10 +4576,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="B2:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R73" sqref="R73"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4568,54 +4587,54 @@
     <col min="1" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="2:2">
+      <c r="B2" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="8" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="8" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="9" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="14:14">
-      <c r="N59" s="8" t="s">
+    <row r="55" spans="10:10">
+      <c r="J55" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="14:14">
-      <c r="N60" s="6" t="s">
+    <row r="56" spans="10:10">
+      <c r="J56" s="6" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="43" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" horizontalDpi="2400" verticalDpi="2400" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>